<commit_message>
replace tuple by a class for the excel reading. Adding the count of number of expected part of a structure
</commit_message>
<xml_diff>
--- a/Plancheck/check_protocol/prostate.xlsx
+++ b/Plancheck/check_protocol/prostate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
   <si>
     <t>Name_of check_protocol</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>vol max</t>
+  </si>
+  <si>
+    <t>Expected part</t>
+  </si>
+  <si>
+    <t>PoumonDt</t>
   </si>
 </sst>
 </file>
@@ -1238,10 +1244,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,11 +1268,17 @@
       <c r="D1" s="8" t="s">
         <v>73</v>
       </c>
+      <c r="E1" s="8" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -1282,6 +1294,9 @@
       <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -1312,6 +1327,9 @@
       </c>
       <c r="D10" s="14">
         <v>5569.9416345124491</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -1371,6 +1389,9 @@
       <c r="D15" s="14">
         <v>560.73982355024589</v>
       </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -1393,6 +1414,9 @@
       <c r="D17" s="14">
         <v>130.38317839653934</v>
       </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
@@ -1401,6 +1425,9 @@
       <c r="A18" s="6" t="s">
         <v>36</v>
       </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
@@ -1415,6 +1442,9 @@
       <c r="D19" s="14">
         <v>309.59451169159098</v>
       </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
@@ -1428,6 +1458,9 @@
       </c>
       <c r="D20" s="14">
         <v>270.90074153704302</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
       </c>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
@@ -1447,6 +1480,9 @@
       <c r="D21" s="14">
         <v>271.54249032790631</v>
       </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
@@ -1459,6 +1495,9 @@
       <c r="A22" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
       <c r="I22" s="13"/>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
@@ -1479,6 +1518,23 @@
       </c>
       <c r="D23" s="14">
         <v>581.80274094704828</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24">
+        <v>50</v>
+      </c>
+      <c r="D24">
+        <v>1500</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1492,10 +1548,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,7 +1559,7 @@
     <col min="1" max="1" width="28.5703125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -1516,78 +1572,81 @@
       <c r="D1" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>54</v>
       </c>
@@ -1662,10 +1721,10 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,7 +1732,7 @@
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -1686,16 +1745,28 @@
       <c r="D1" s="12" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>67</v>
       </c>
       <c r="B2">
         <v>-1000</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>68</v>
       </c>
@@ -1703,15 +1774,18 @@
         <v>-300</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>71</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
check number of parts AND check missing slices.
</commit_message>
<xml_diff>
--- a/Plancheck/check_protocol/prostate.xlsx
+++ b/Plancheck/check_protocol/prostate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -779,10 +779,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1110,7 +1114,7 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,13 +1250,14 @@
   </sheetPr>
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1276,9 +1281,6 @@
       <c r="A2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -1294,9 +1296,6 @@
       <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -1322,189 +1321,165 @@
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="12">
         <v>112.02</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="12">
         <v>5569.9416345124491</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="12">
         <v>39.14</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="12">
         <v>560.73982355024589</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="12">
         <v>30.94</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="12">
         <v>130.38317839653934</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="12">
         <v>9.1</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="12">
         <v>309.59451169159098</v>
       </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="12">
         <v>96.808165954476038</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="12">
         <v>270.90074153704302</v>
       </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="12">
         <v>100.38</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="12">
         <v>271.54249032790631</v>
       </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
@@ -1513,14 +1488,11 @@
       <c r="B23">
         <v>0</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="12">
         <v>91.37</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="12">
         <v>581.80274094704828</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -1557,6 +1529,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1572,7 +1545,7 @@
       <c r="D1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="10" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1723,29 +1696,30 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="14" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1756,15 +1730,6 @@
       <c r="B2">
         <v>-1000</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -1780,9 +1745,6 @@
       </c>
       <c r="B4">
         <v>0</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
robust reading of xlsx (grrr.)
</commit_message>
<xml_diff>
--- a/Plancheck/check_protocol/prostate.xlsx
+++ b/Plancheck/check_protocol/prostate.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="79">
   <si>
     <t>Name_of check_protocol</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1268,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,6 +1395,9 @@
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>4</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="C17" s="14">
         <v>30.94</v>

</xml_diff>

<commit_message>
check dose objective : dose mean ok
</commit_message>
<xml_diff>
--- a/Plancheck/check_protocol/prostate.xlsx
+++ b/Plancheck/check_protocol/prostate.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
     <sheet name="Clinical Structures" sheetId="2" r:id="rId2"/>
     <sheet name="opt structures" sheetId="3" r:id="rId3"/>
     <sheet name="couch_structures" sheetId="4" r:id="rId4"/>
+    <sheet name="Doses" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="93">
   <si>
     <t>Name_of check_protocol</t>
   </si>
@@ -256,6 +257,51 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>Contrainte 1</t>
+  </si>
+  <si>
+    <t>Contrainte 2</t>
+  </si>
+  <si>
+    <t>Contrainte 3</t>
+  </si>
+  <si>
+    <t>Contrainte 4</t>
+  </si>
+  <si>
+    <t>Contrainte 5</t>
+  </si>
+  <si>
+    <t>Contrainte 6</t>
+  </si>
+  <si>
+    <t>Contrainte 7</t>
+  </si>
+  <si>
+    <t>Contrainte 8</t>
+  </si>
+  <si>
+    <t>Contrainte 9</t>
+  </si>
+  <si>
+    <t>Contrainte 10</t>
+  </si>
+  <si>
+    <t>mean&lt;45,5Gy</t>
+  </si>
+  <si>
+    <t>,,,</t>
+  </si>
+  <si>
+    <t>V20Gy&lt;45,5Gy</t>
+  </si>
+  <si>
+    <t>CTV sein</t>
+  </si>
+  <si>
+    <t>mean&gt;20,1Gy</t>
   </si>
 </sst>
 </file>
@@ -398,7 +444,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -600,6 +646,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -763,7 +815,7 @@
     <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -783,6 +835,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -801,6 +854,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1264,217 +1319,217 @@
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" activeCellId="1" sqref="A15:A23 A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="13" customWidth="1"/>
-    <col min="2" max="4" width="11.42578125" style="14"/>
-    <col min="5" max="5" width="15.42578125" style="14" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="14"/>
+    <col min="1" max="1" width="16.42578125" style="14" customWidth="1"/>
+    <col min="2" max="4" width="11.42578125" style="15"/>
+    <col min="5" max="5" width="15.42578125" style="15" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="13" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="15">
         <v>112.02</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="15">
         <v>5569.9416345124491</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="15">
         <v>39.14</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="15">
         <v>560.73982355024589</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="15">
         <v>30.94</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="15">
         <v>130.38317839653934</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="15">
         <v>9.1</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="15">
         <v>309.59451169159098</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="15">
         <v>96.808165954476038</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="15">
         <v>270.90074153704302</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="15">
         <v>1</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="15" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="15">
         <v>100.38</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="15">
         <v>271.54249032790631</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="15">
         <v>1</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="15" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="15">
         <v>0</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="15">
         <v>91.37</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="15">
         <v>581.80274094704828</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1678,23 +1733,23 @@
     <col min="5" max="5" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1733,4 +1788,129 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="11" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
first version works with Dxx% and Vxx% all units (Gy,cc,%)
</commit_message>
<xml_diff>
--- a/Plancheck/check_protocol/prostate.xlsx
+++ b/Plancheck/check_protocol/prostate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="101">
   <si>
     <t>Name_of check_protocol</t>
   </si>
@@ -295,13 +295,37 @@
     <t>,,,</t>
   </si>
   <si>
-    <t>V20Gy&lt;45,5Gy</t>
+    <t>mean&lt;20,1Gy</t>
   </si>
   <si>
     <t>CTV sein</t>
   </si>
   <si>
-    <t>mean&gt;20,1Gy</t>
+    <t>V20,0Gy&lt;30cc</t>
+  </si>
+  <si>
+    <t>V20,0Gy&lt;45,2cc</t>
+  </si>
+  <si>
+    <t>D20%&lt;45Gy</t>
+  </si>
+  <si>
+    <t>V20Gy&lt;10%</t>
+  </si>
+  <si>
+    <t>V10%&lt;5%</t>
+  </si>
+  <si>
+    <t>V15,5%&lt;5,8cc</t>
+  </si>
+  <si>
+    <t>D10%&lt;5%</t>
+  </si>
+  <si>
+    <t>D100cc&gt;1%</t>
+  </si>
+  <si>
+    <t>D100cc&gt;1Gy</t>
   </si>
 </sst>
 </file>
@@ -815,7 +839,7 @@
     <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -856,6 +880,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1798,13 +1823,15 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="11" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="11" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -1873,7 +1900,7 @@
         <v>88</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1901,12 +1928,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B12" t="s">
-        <v>92</v>
+      <c r="B12" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
try/catch to debug the case of old tomo "0 beam" plans
</commit_message>
<xml_diff>
--- a/Plancheck/check_protocol/prostate.xlsx
+++ b/Plancheck/check_protocol/prostate.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="113">
   <si>
     <t>Name_of check_protocol</t>
   </si>
@@ -328,9 +328,6 @@
     <t>D100cc&gt;1Gy</t>
   </si>
   <si>
-    <t>Energy</t>
-  </si>
-  <si>
     <t>6X</t>
   </si>
   <si>
@@ -350,6 +347,21 @@
   </si>
   <si>
     <t>12E</t>
+  </si>
+  <si>
+    <t>CQ</t>
+  </si>
+  <si>
+    <t>PDIP</t>
+  </si>
+  <si>
+    <t>Octa4D</t>
+  </si>
+  <si>
+    <t>RUBY</t>
+  </si>
+  <si>
+    <t>Energie des faisceaux</t>
   </si>
 </sst>
 </file>
@@ -1248,15 +1260,16 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="37" style="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="15.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="1" customWidth="1"/>
     <col min="6" max="8" width="9.140625" style="1"/>
     <col min="9" max="9" width="3" style="4" customWidth="1"/>
     <col min="10" max="11" width="9.140625" style="1"/>
@@ -1349,13 +1362,22 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="L9" s="19" t="s">
         <v>19</v>
       </c>
@@ -1367,44 +1389,59 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L12" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L13" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L14" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L15" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L16" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L17" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L18" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L20" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L21" s="19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L22" s="19" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G39" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
       <formula1>$L$6:$L$7</formula1>
     </dataValidation>
@@ -1416,6 +1453,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
       <formula1>$L$12:$L$18</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9 C9 D9">
+      <formula1>$L$20:$L$22</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
export to pdf v1
</commit_message>
<xml_diff>
--- a/Plancheck/check_protocol/prostate.xlsx
+++ b/Plancheck/check_protocol/prostate.xlsx
@@ -1310,9 +1310,7 @@
   </sheetPr>
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Add Mandatory column to structures
</commit_message>
<xml_diff>
--- a/Plancheck/check_protocol/prostate.xlsx
+++ b/Plancheck/check_protocol/prostate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21480" windowHeight="5400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21480" windowHeight="5400" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="160">
   <si>
     <t>Name_of check_protocol</t>
   </si>
@@ -628,6 +628,15 @@
   </si>
   <si>
     <t>3.0</t>
+  </si>
+  <si>
+    <t>Mandatory</t>
+  </si>
+  <si>
+    <t>oui</t>
+  </si>
+  <si>
+    <t>manque</t>
   </si>
 </sst>
 </file>
@@ -1538,8 +1547,8 @@
   </sheetPr>
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1966,10 +1975,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" activeCellId="1" sqref="A15:A23 A13"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1980,7 +1989,7 @@
     <col min="6" max="16384" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
@@ -1999,48 +2008,51 @@
       <c r="F1" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>30</v>
       </c>
@@ -2053,23 +2065,26 @@
       <c r="E10" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>33</v>
       </c>
@@ -2077,7 +2092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>34</v>
       </c>
@@ -2087,13 +2102,16 @@
       <c r="D15" s="15">
         <v>560.73982355024589</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
@@ -2106,13 +2124,16 @@
       <c r="E17" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>37</v>
       </c>
@@ -2122,8 +2143,11 @@
       <c r="D19" s="15">
         <v>309.59451169159098</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>38</v>
       </c>
@@ -2139,8 +2163,11 @@
       <c r="F20" s="15" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>39</v>
       </c>
@@ -2156,8 +2183,11 @@
       <c r="F21" s="15" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>40</v>
       </c>
@@ -2165,7 +2195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>3</v>
       </c>
@@ -2180,6 +2210,9 @@
       </c>
       <c r="E23" s="15">
         <v>1</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2193,10 +2226,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,7 +2238,7 @@
     <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -2224,140 +2257,163 @@
       <c r="F1" s="8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>66</v>
+      </c>
+      <c r="G28" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G29" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2370,10 +2426,10 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2382,7 +2438,7 @@
     <col min="5" max="5" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
@@ -2401,37 +2457,52 @@
       <c r="F1" s="11" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>67</v>
       </c>
       <c r="B2">
         <v>-1000</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>68</v>
       </c>
       <c r="B3">
         <v>-300</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>71</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B5">
         <v>-900</v>
+      </c>
+      <c r="G5" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
check protocol sein and sein hypo
</commit_message>
<xml_diff>
--- a/Plancheck/check_protocol/prostate.xlsx
+++ b/Plancheck/check_protocol/prostate.xlsx
@@ -799,7 +799,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1012,6 +1012,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1176,21 +1182,12 @@
     <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1220,6 +1217,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1548,392 +1569,559 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20" style="1" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="3" style="4" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="20" style="12" customWidth="1"/>
+    <col min="6" max="8" width="9.140625" style="12"/>
+    <col min="9" max="9" width="3" style="2" customWidth="1"/>
     <col min="10" max="11" width="9.140625" style="1"/>
-    <col min="12" max="12" width="41.28515625" style="19" customWidth="1"/>
+    <col min="12" max="12" width="41.28515625" style="16" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="19" t="s">
         <v>2</v>
       </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="19">
         <v>2.5</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
+      <c r="L2" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="19">
         <v>0.125</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="19">
         <v>0.125</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="G3" s="19"/>
+      <c r="H3" s="20"/>
+      <c r="L3" s="16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="19">
         <v>1.25</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="20"/>
+      <c r="L4" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="22">
         <v>1</v>
       </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="20"/>
+      <c r="L6" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="20"/>
+      <c r="L7" s="16" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="19" t="s">
         <v>102</v>
       </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="19" t="s">
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="20"/>
+      <c r="L9" s="16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="L10" s="19" t="s">
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
+      <c r="L10" s="16" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
+    </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="19">
         <v>300</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="19">
         <v>3</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="19">
         <v>100</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="19">
         <v>30</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="19">
         <v>0.1</v>
       </c>
-      <c r="L12" s="19" t="s">
+      <c r="H12" s="20"/>
+      <c r="L12" s="16" t="s">
         <v>101</v>
       </c>
     </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20"/>
+    </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="L14" s="19" t="s">
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="20"/>
+      <c r="L14" s="16" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L15" s="19" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="20"/>
+      <c r="L15" s="16" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="20"/>
+      <c r="L16" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="B17" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="L16" s="19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="20"/>
+      <c r="L17" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="B18" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="L17" s="19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="20"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
+      <c r="L18" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="B19" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="L18" s="19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="20"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="20"/>
+      <c r="L19" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="B20" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="L19" s="19" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="20"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="20"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="B21" s="19" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="20"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="20"/>
+      <c r="L21" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="B22" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="L21" s="19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="20"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="20"/>
+      <c r="L22" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="B23" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="L22" s="19" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="20"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="20"/>
+      <c r="L23" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="B24" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="L23" s="19" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="20"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="20"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="B25" s="19" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="20"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="20"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="C25" s="1">
+      <c r="B26" s="19">
         <v>200</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="20"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="20"/>
+      <c r="L26" s="16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="C26" s="1">
+      <c r="B27" s="19">
         <v>200</v>
       </c>
-      <c r="L26" s="19" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="20"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="20"/>
+      <c r="L27" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="B28" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="L27" s="19" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L28" s="19" t="s">
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="L28" s="16" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L29" s="19" t="s">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L29" s="16" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L30" s="19" t="s">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L30" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L31" s="19" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L31" s="16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L32" s="19" t="s">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L32" s="16" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="33" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L33" s="19" t="s">
+      <c r="L33" s="16" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="34" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L34" s="19" t="s">
+      <c r="L34" s="16" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="35" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L35" s="19" t="s">
+      <c r="L35" s="16" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="36" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L36" s="19" t="s">
+      <c r="L36" s="16" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="37" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L37" s="19" t="s">
+      <c r="L37" s="16" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="38" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L38" s="19" t="s">
+      <c r="L38" s="16" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="39" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L39" s="19" t="s">
+      <c r="L39" s="16" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="40" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G40" s="5"/>
-      <c r="L40" s="19" t="s">
+      <c r="G40" s="23"/>
+      <c r="L40" s="16" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="41" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L41" s="19" t="s">
+      <c r="L41" s="16" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="43" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L43" s="19" t="s">
+      <c r="L43" s="16" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="44" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L44" s="19" t="s">
+      <c r="L44" s="16" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="46" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L46" s="19" t="s">
+      <c r="L46" s="16" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="47" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="L47" s="19" t="s">
+      <c r="L47" s="16" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1983,235 +2171,235 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="14" customWidth="1"/>
-    <col min="2" max="4" width="11.42578125" style="15"/>
-    <col min="5" max="5" width="15.42578125" style="15" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="15"/>
+    <col min="1" max="1" width="16.42578125" style="11" customWidth="1"/>
+    <col min="2" max="4" width="11.42578125" style="12"/>
+    <col min="5" max="5" width="15.42578125" style="12" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="10" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="12">
         <v>112.02</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="12">
         <v>5569.9416345124491</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="12">
         <v>1</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="12" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="12">
         <v>39.14</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="12">
         <v>560.73982355024589</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="12" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="11" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="12">
         <v>30.94</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="12">
         <v>130.38317839653934</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="12">
         <v>1</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="12" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="11" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="12">
         <v>9.1</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="12">
         <v>309.59451169159098</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="12" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="12">
         <v>96.808165954476038</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="12">
         <v>270.90074153704302</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="12">
         <v>1</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="12" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="12">
         <v>100.38</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="12">
         <v>271.54249032790631</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="12">
         <v>1</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="12" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="12">
         <v>0</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="12">
         <v>91.37</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="12">
         <v>581.80274094704828</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="12">
         <v>1</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="12" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2234,55 +2422,55 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="5" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>45</v>
       </c>
       <c r="G6" t="s">
@@ -2290,7 +2478,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>46</v>
       </c>
       <c r="G7" t="s">
@@ -2298,82 +2486,82 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="3" t="s">
         <v>61</v>
       </c>
       <c r="G23" t="s">
@@ -2381,27 +2569,27 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="3" t="s">
         <v>66</v>
       </c>
       <c r="G28" t="s">
@@ -2409,7 +2597,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="3" t="s">
         <v>159</v>
       </c>
       <c r="G29" t="s">
@@ -2429,7 +2617,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2438,31 +2626,31 @@
     <col min="5" max="5" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="8" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B2">
@@ -2473,7 +2661,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B3">
@@ -2484,7 +2672,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B4">
@@ -2495,7 +2683,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B5">
@@ -2529,129 +2717,129 @@
     <col min="4" max="11" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="14" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B6" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="11" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="I12" s="18" t="s">
+      <c r="I12" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="15" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tested on 6 prostates ; remove useless tests
</commit_message>
<xml_diff>
--- a/Plancheck/check_protocol/prostate.xlsx
+++ b/Plancheck/check_protocol/prostate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21480" windowHeight="5400" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21480" windowHeight="5400" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="160">
   <si>
     <t>Name_of check_protocol</t>
   </si>
@@ -423,45 +423,9 @@
     <t>Contrainte 10</t>
   </si>
   <si>
-    <t>mean&lt;45,5Gy</t>
-  </si>
-  <si>
     <t>,,,</t>
   </si>
   <si>
-    <t>mean&lt;20,1Gy</t>
-  </si>
-  <si>
-    <t>CTV sein</t>
-  </si>
-  <si>
-    <t>V20,0Gy&lt;30cc</t>
-  </si>
-  <si>
-    <t>V20,0Gy&lt;45,2cc</t>
-  </si>
-  <si>
-    <t>D20%&lt;45Gy</t>
-  </si>
-  <si>
-    <t>V20Gy&lt;10%</t>
-  </si>
-  <si>
-    <t>V10%&lt;5%</t>
-  </si>
-  <si>
-    <t>V15,5%&lt;5,8cc</t>
-  </si>
-  <si>
-    <t>D10%&lt;5%</t>
-  </si>
-  <si>
-    <t>D100cc&gt;1%</t>
-  </si>
-  <si>
-    <t>D100cc&gt;1Gy</t>
-  </si>
-  <si>
     <t>6X</t>
   </si>
   <si>
@@ -558,9 +522,6 @@
     <t>Manual</t>
   </si>
   <si>
-    <t>Jaw Tracking</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
@@ -637,6 +598,45 @@
   </si>
   <si>
     <t>manque</t>
+  </si>
+  <si>
+    <t>D95%&gt;95%</t>
+  </si>
+  <si>
+    <t>D1cc&lt;72,4Gy</t>
+  </si>
+  <si>
+    <t>D0,1cc&lt;73,5Gy</t>
+  </si>
+  <si>
+    <t>V58Gy&lt;50%</t>
+  </si>
+  <si>
+    <t>V67Gy&lt;25%</t>
+  </si>
+  <si>
+    <t>V71Gy&lt;5%</t>
+  </si>
+  <si>
+    <t>D0,1cc&lt;74,8Gy</t>
+  </si>
+  <si>
+    <t>mean&lt;45Gy</t>
+  </si>
+  <si>
+    <t>V55Gy&lt;5%</t>
+  </si>
+  <si>
+    <t>D0,1cc&lt;59Gy</t>
+  </si>
+  <si>
+    <t>V15Gy&lt;830cc</t>
+  </si>
+  <si>
+    <t>V45Gy&lt;150cc</t>
+  </si>
+  <si>
+    <t>Jaw Tracking (NOVA)</t>
   </si>
 </sst>
 </file>
@@ -1569,7 +1569,7 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1709,10 +1709,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -1723,10 +1723,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -1740,10 +1740,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
@@ -1766,10 +1766,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C12" s="19">
         <v>300</v>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="H12" s="20"/>
       <c r="L12" s="16" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1802,10 +1802,10 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -1814,7 +1814,7 @@
       <c r="G14" s="19"/>
       <c r="H14" s="20"/>
       <c r="L14" s="16" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1826,12 +1826,12 @@
       <c r="G15" s="19"/>
       <c r="H15" s="20"/>
       <c r="L15" s="16" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="20"/>
@@ -1841,15 +1841,15 @@
       <c r="G16" s="19"/>
       <c r="H16" s="20"/>
       <c r="L16" s="16" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="19"/>
@@ -1858,15 +1858,15 @@
       <c r="G17" s="19"/>
       <c r="H17" s="20"/>
       <c r="L17" s="16" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="19"/>
@@ -1875,15 +1875,15 @@
       <c r="G18" s="19"/>
       <c r="H18" s="20"/>
       <c r="L18" s="16" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="19"/>
@@ -1892,15 +1892,15 @@
       <c r="G19" s="19"/>
       <c r="H19" s="20"/>
       <c r="L19" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="19"/>
@@ -1911,10 +1911,10 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="19"/>
@@ -1923,15 +1923,15 @@
       <c r="G21" s="19"/>
       <c r="H21" s="20"/>
       <c r="L21" s="16" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="19"/>
@@ -1940,15 +1940,15 @@
       <c r="G22" s="19"/>
       <c r="H22" s="20"/>
       <c r="L22" s="16" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>143</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>156</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="19"/>
@@ -1957,15 +1957,15 @@
       <c r="G23" s="19"/>
       <c r="H23" s="20"/>
       <c r="L23" s="16" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="19"/>
@@ -1976,10 +1976,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="C25" s="20"/>
       <c r="D25" s="19"/>
@@ -1990,7 +1990,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B26" s="19">
         <v>200</v>
@@ -2002,12 +2002,12 @@
       <c r="G26" s="19"/>
       <c r="H26" s="20"/>
       <c r="L26" s="16" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="B27" s="19">
         <v>200</v>
@@ -2019,15 +2019,15 @@
       <c r="G27" s="19"/>
       <c r="H27" s="20"/>
       <c r="L27" s="16" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
@@ -2036,93 +2036,93 @@
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
       <c r="L28" s="16" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L29" s="16" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L30" s="16" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L31" s="16" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L32" s="16" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="7:12" x14ac:dyDescent="0.25">
       <c r="L33" s="16" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="7:12" x14ac:dyDescent="0.25">
       <c r="L34" s="16" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="7:12" x14ac:dyDescent="0.25">
       <c r="L35" s="16" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="7:12" x14ac:dyDescent="0.25">
       <c r="L36" s="16" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="7:12" x14ac:dyDescent="0.25">
       <c r="L37" s="16" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="7:12" x14ac:dyDescent="0.25">
       <c r="L38" s="16" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="7:12" x14ac:dyDescent="0.25">
       <c r="L39" s="16" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G40" s="23"/>
       <c r="L40" s="16" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="7:12" x14ac:dyDescent="0.25">
       <c r="L41" s="16" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="7:12" x14ac:dyDescent="0.25">
       <c r="L43" s="16" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="7:12" x14ac:dyDescent="0.25">
       <c r="L44" s="16" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="7:12" x14ac:dyDescent="0.25">
       <c r="L46" s="16" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="7:12" x14ac:dyDescent="0.25">
       <c r="L47" s="16" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2166,7 +2166,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2197,7 +2197,7 @@
         <v>75</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2254,7 +2254,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2276,9 +2276,6 @@
       <c r="A14" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="12">
-        <v>1</v>
-      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -2291,7 +2288,7 @@
         <v>560.73982355024589</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2313,7 +2310,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2332,7 +2329,7 @@
         <v>309.59451169159098</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2352,7 +2349,7 @@
         <v>76</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2372,7 +2369,7 @@
         <v>77</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2400,7 +2397,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2416,8 +2413,8 @@
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2446,7 +2443,7 @@
         <v>75</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2474,7 +2471,7 @@
         <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2482,7 +2479,7 @@
         <v>46</v>
       </c>
       <c r="G7" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2565,7 +2562,7 @@
         <v>61</v>
       </c>
       <c r="G23" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2593,15 +2590,12 @@
         <v>66</v>
       </c>
       <c r="G28" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G29" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2616,7 +2610,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -2646,7 +2640,7 @@
         <v>75</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2657,7 +2651,7 @@
         <v>-1000</v>
       </c>
       <c r="G2" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2668,7 +2662,7 @@
         <v>-300</v>
       </c>
       <c r="G3" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2679,7 +2673,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2690,7 +2684,7 @@
         <v>-900</v>
       </c>
       <c r="G5" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2705,8 +2699,8 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2752,7 +2746,7 @@
         <v>87</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2764,6 +2758,9 @@
       <c r="A3" s="11" t="s">
         <v>34</v>
       </c>
+      <c r="B3" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -2774,17 +2771,27 @@
       <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
@@ -2795,11 +2802,17 @@
       <c r="A8" s="11" t="s">
         <v>38</v>
       </c>
+      <c r="B8" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>39</v>
       </c>
+      <c r="B9" s="6" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -2810,37 +2823,31 @@
       <c r="A11" s="11" t="s">
         <v>3</v>
       </c>
+      <c r="B11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="12" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>90</v>
+        <v>156</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>95</v>
+        <v>157</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>100</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaner : do not check useless checks for tomo
</commit_message>
<xml_diff>
--- a/Plancheck/check_protocol/prostate.xlsx
+++ b/Plancheck/check_protocol/prostate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21480" windowHeight="5400" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21480" windowHeight="5400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -2165,8 +2165,8 @@
   </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2250,9 +2250,6 @@
       <c r="D10" s="12">
         <v>5569.9416345124491</v>
       </c>
-      <c r="E10" s="12">
-        <v>1</v>
-      </c>
       <c r="G10" s="12" t="s">
         <v>145</v>
       </c>
@@ -2286,6 +2283,9 @@
       </c>
       <c r="D15" s="12">
         <v>560.73982355024589</v>
+      </c>
+      <c r="E15" s="12">
+        <v>1</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>145</v>
@@ -2413,8 +2413,8 @@
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2455,6 +2455,9 @@
       <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -2470,14 +2473,14 @@
       <c r="A6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G6" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>46</v>
       </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
       <c r="G7" t="s">
         <v>145</v>
       </c>
@@ -2490,6 +2493,9 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>